<commit_message>
Added sd-login and word doc
</commit_message>
<xml_diff>
--- a/Theoretical/requirements.xlsx
+++ b/Theoretical/requirements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obarilan\Documents\University\BACkUP-18.4-1930\Analysis-Design\part A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obarilan\Documents\University\Analysis-Design-2\Theoretical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="188">
   <si>
     <t>תאור הדרישה</t>
   </si>
@@ -113,15 +113,9 @@
     <t>הוספת בית עסק תתאפשר ע"י מנהל מערכת בלבד.</t>
   </si>
   <si>
-    <t>המערכת תתמוך בהוספת בתי עסק למימוש קופונים (שם, כתובת, עיר, תיאור, קטגוריה).</t>
-  </si>
-  <si>
     <t>הוספת קופון מרשת חברתית תתאפשר ע"י כל משתמש שנרשם למערכת.</t>
   </si>
   <si>
-    <t>המערכת תשמור את הקופונים הקיימים במערכת עד לשנה לאחר תאריך המימוש האחרון.</t>
-  </si>
-  <si>
     <t>צפייה בפרטי הזמנות</t>
   </si>
   <si>
@@ -155,21 +149,12 @@
     <t>המערכת תתמוך בהזמנת קופונים מבתי עסק ע"י משתמשים רשומים במערכת.</t>
   </si>
   <si>
-    <t>משתמש אשר מחובר למערכת, יוכל לבצע הזמנה של קופון עד לתאריך המימוש האחרון של הקופון.</t>
-  </si>
-  <si>
     <t>תהליך הזמנת הקופון יתבצע באופן מאובטח.</t>
   </si>
   <si>
-    <t>המשתמש יקבל התראה מהמערכת על קופונים שרכש אך עדיין לא מימש, כשבוע לפני התאריך האחרון למימוש.</t>
-  </si>
-  <si>
     <t>מימוש קופון</t>
   </si>
   <si>
-    <t>בעת הגעת המשתמש לבית העסק למימוש הקופון, יזין בית העסק את הקוד שקיבל המשתמש לשם זיהוי ואישור סופי של מימוש הקופון.</t>
-  </si>
-  <si>
     <t>1.1.1</t>
   </si>
   <si>
@@ -302,9 +287,6 @@
     <t>מנהלי מערכת יאשרו קופונים שהוזנו ע"י משתמשים ובתי עסק.</t>
   </si>
   <si>
-    <t>משתמש שמימש קופון יוכל לדרגו (1-5) בכל עת ובכך להבטיח את אמינות הקופון ובית העסק.</t>
-  </si>
-  <si>
     <t>סולם ערכים (1- לא קריטי, 5-קריטי)</t>
   </si>
   <si>
@@ -335,9 +317,6 @@
     <t xml:space="preserve">המערכת תתמוך בחיפוש קופונים ע"י משתמשים ובעלי עסק. </t>
   </si>
   <si>
-    <t>משתמש יוכל לבצע חיפוש של קופון לפי מיקומו וכן לפי בתי עסק וקטגוריות (מסעדות, פנאי ובילוי, צרכנות וכו').</t>
-  </si>
-  <si>
     <t>1.4.3</t>
   </si>
   <si>
@@ -362,27 +341,15 @@
     <t>5.1.4</t>
   </si>
   <si>
-    <t>משתמש יוכל לבצע חיפוש של בית עסק לפי מיקומו וכן לפי קטגוריות (מסעדות, פנאי ובילוי, צרכנות וכו').</t>
-  </si>
-  <si>
     <t>עריכת פרטי בית העסק תתאפשר ע"י בית העסק בלבד.</t>
   </si>
   <si>
-    <t>המערכת תתמוך בהוספת קופון (שם, תיאור, קטגוריה, מחיר מקורי, מחיר לאחר הנחה, דירוג, תאריך אחרון למימוש) עבור בית עסק מסוים.</t>
-  </si>
-  <si>
-    <t>לאחר אישור של מנהל המערכת על הוספת הקופון, המשתמש יקבל התראה על קופונים לאור המיקום ו/או העדפות המשתמש.</t>
-  </si>
-  <si>
     <t>מנהלי מערכת יוסיפו בעלי עסקים למערכת.</t>
   </si>
   <si>
     <t>המערכת תתמוך בבעל עסק אחד לכל בית עסק.</t>
   </si>
   <si>
-    <t>לאחר הזמנת הקופון וביצוע תשלום על ההזמנה, יקבל המשתמש קוד מיוחד (serial key) וקבלה למייל המאשרת את הזמנתו.</t>
-  </si>
-  <si>
     <t>לאחר הזמנת הקופון, יוכל המשתמש לצפות בקופון/ים שהזמין.</t>
   </si>
   <si>
@@ -455,9 +422,6 @@
     <t>ייעול שמירת נתונים</t>
   </si>
   <si>
-    <t>יישום אינדקסים על חלק מהטבלאות לייעול זמני חיפוש</t>
-  </si>
-  <si>
     <t>מנתח מערכת</t>
   </si>
   <si>
@@ -476,18 +440,9 @@
     <t>9.1.1</t>
   </si>
   <si>
-    <t>אם המנגון מכוון למצב התראת מיקום, המשתמש יקבל התראה על קופון הנמצא בקרבתו.</t>
-  </si>
-  <si>
-    <t>אם המנגנון מכוון למצב העדפה, המשתמש יקבל התראה על קופון לפי קטגוריות שהזין בעת הרשמתו למערכת.</t>
-  </si>
-  <si>
     <t>5.1.5</t>
   </si>
   <si>
-    <t>אם המנגנון מכוון למצב משולב, המשתמש יקבל התראה על קופון לפי קטגוריות שהזין בעת הרשמתו למערכת ובתנאי שמועד הקופון סמוך לשעה הנוכחית.</t>
-  </si>
-  <si>
     <t>5.3.1</t>
   </si>
   <si>
@@ -512,24 +467,15 @@
     <t>5.3.3</t>
   </si>
   <si>
-    <t>בעת מעבר ממצב כבוי למצב דלוק, המערכת תזכור את העדפת המשתמש מהפעם האחרונה שהיתה דלוקה.</t>
-  </si>
-  <si>
     <t>5.1.6</t>
   </si>
   <si>
-    <t>הצגת ההתראה תיהיה 10 שניות או עד שהמשתמש לוחץ "סגור" (הראשון מהשניים)</t>
-  </si>
-  <si>
     <t>7.2.1</t>
   </si>
   <si>
     <t>5.1.7</t>
   </si>
   <si>
-    <t>לאחר שנוספו 10 קופונים חדשים מרגע הפעלת המערכת, הם מוצגים למשתמש בתנאי שהמערכת אינה מציגה קופונים כעת</t>
-  </si>
-  <si>
     <t>הגבלת התראות</t>
   </si>
   <si>
@@ -576,6 +522,90 @@
   </si>
   <si>
     <t>המערכת תכבה את עצמה לאחר 5 נסיונות התחברות כושלים רצופים.</t>
+  </si>
+  <si>
+    <t>7.1.1.1</t>
+  </si>
+  <si>
+    <t>נתוני המערכת יישמרו על חומרה שונה מזו של הלקוח</t>
+  </si>
+  <si>
+    <t>7.1.1.2</t>
+  </si>
+  <si>
+    <t>תוכנת הלקוח תיגש (תקרא ותכתוב) לנתונים בבסיס נתונים מרוחק</t>
+  </si>
+  <si>
+    <t>המערכת תתמוך בהוספת קופון (שם, תיאור, קטגוריה, מחיר מקורי,
+ מחיר לאחר הנחה, דירוג, תאריך אחרון למימוש) עבור בית עסק מסוים.</t>
+  </si>
+  <si>
+    <t>לאחר אישור של מנהל המערכת על הוספת הקופון, המשתמש יקבל התראה 
+על קופונים לאור המיקום ו/או העדפות המשתמש.</t>
+  </si>
+  <si>
+    <t>המערכת תשמור את הקופונים הקיימים במערכת עד לשנה לאחר תאריך 
+המימוש האחרון.</t>
+  </si>
+  <si>
+    <t>משתמש יוכל לבצע חיפוש של קופון לפי מיקומו וכן לפי בתי עסק וקטגוריות
+ (מסעדות, פנאי ובילוי, צרכנות וכו').</t>
+  </si>
+  <si>
+    <t>המערכת תתמוך בהוספת בתי עסק למימוש קופונים
+ (שם, כתובת, עיר, תיאור, קטגוריה).</t>
+  </si>
+  <si>
+    <t>משתמש יוכל לבצע חיפוש של בית עסק לפי מיקומו וכן 
+לפי קטגוריות (מסעדות, פנאי ובילוי, צרכנות וכו').</t>
+  </si>
+  <si>
+    <t>משתמש אשר מחובר למערכת, יוכל לבצע הזמנה של קופון עד 
+לתאריך המימוש האחרון של הקופון.</t>
+  </si>
+  <si>
+    <t>לאחר הזמנת הקופון וביצוע תשלום על ההזמנה, יקבל המשתמש קוד 
+מיוחד (serial key) וקבלה למייל המאשרת את הזמנתו.</t>
+  </si>
+  <si>
+    <t>בעת הגעת המשתמש לבית העסק למימוש הקופון, יזין בית העסק את 
+הקוד שקיבל המשתמש לשם זיהוי ואישור סופי של מימוש הקופון.</t>
+  </si>
+  <si>
+    <t>משתמש שמימש קופון יוכל לדרגו (1-5) בכל עת ובכך להבטיח את 
+אמינות הקופון ובית העסק.</t>
+  </si>
+  <si>
+    <t>אם המנגון מכוון למצב התראת מיקום, המשתמש יקבל התראה על קופון
+ הנמצא בקרבתו.</t>
+  </si>
+  <si>
+    <t>אם המנגנון מכוון למצב העדפה, המשתמש יקבל התראה על קופון לפי
+ קטגוריות שהזין בעת הרשמתו למערכת.</t>
+  </si>
+  <si>
+    <t>אם המנגנון מכוון למצב משולב, המשתמש יקבל התראה על קופון
+ לפי קטגוריות שהזין בעת הרשמתו למערכת ובתנאי שמועד הקופון סמוך לשעה הנוכחית.</t>
+  </si>
+  <si>
+    <t>הצגת ההתראה תיהיה 10 שניות או עד שהמשתמש לוחץ "סגור" 
+(הראשון מהשניים)</t>
+  </si>
+  <si>
+    <t>לאחר שנוספו 10 קופונים חדשים מרגע הפעלת המערכת, הם 
+מוצגים למשתמש בתנאי שהמערכת אינה מציגה קופונים כעת</t>
+  </si>
+  <si>
+    <t>המשתמש יקבל התראה מהמערכת על קופונים שרכש אך עדיין 
+לא מימש, כשבוע לפני התאריך האחרון למימוש.</t>
+  </si>
+  <si>
+    <t>בעת מעבר ממצב כבוי למצב דלוק, המערכת תזכור את העדפת 
+המשתמש מהפעם האחרונה שהיתה דלוקה.</t>
+  </si>
+  <si>
+    <t>נתוני המערכת יישמרו בצורה שתייעל זמני חיפוש (יישום אינדקסים
+ על חלק מהטבלאות)</t>
   </si>
 </sst>
 </file>
@@ -690,7 +720,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -708,6 +738,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
@@ -1140,21 +1176,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A51" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="158.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="83.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
     <col min="8" max="8" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" customWidth="1"/>
   </cols>
@@ -1182,10 +1218,10 @@
         <v>7</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75">
@@ -1201,25 +1237,25 @@
     </row>
     <row r="3" spans="1:9" ht="70.5" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -1235,9 +1271,9 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75">
+    <row r="5" spans="1:9" ht="37.5">
       <c r="A5" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -1245,14 +1281,14 @@
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>114</v>
+      <c r="D5" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G5" s="3">
         <v>5</v>
@@ -1260,9 +1296,9 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="37.5">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
@@ -1270,14 +1306,14 @@
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>115</v>
+      <c r="D6" s="15" t="s">
+        <v>171</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -1287,7 +1323,7 @@
     </row>
     <row r="7" spans="1:9" ht="18.75">
       <c r="A7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -1296,13 +1332,13 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G7" s="3">
         <v>5</v>
@@ -1310,9 +1346,9 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" ht="18.75">
+    <row r="8" spans="1:9" ht="37.5">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -1320,14 +1356,14 @@
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
+      <c r="D8" s="15" t="s">
+        <v>172</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G8" s="3">
         <v>2</v>
@@ -1337,7 +1373,7 @@
     </row>
     <row r="9" spans="1:9" ht="18.75">
       <c r="A9" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -1346,13 +1382,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G9" s="3">
         <v>3</v>
@@ -1362,7 +1398,7 @@
     </row>
     <row r="10" spans="1:9" ht="18.75">
       <c r="A10" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -1371,13 +1407,13 @@
         <v>16</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G10" s="3">
         <v>5</v>
@@ -1387,22 +1423,22 @@
     </row>
     <row r="11" spans="1:9" ht="18.75">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G11" s="3">
         <v>4</v>
@@ -1412,22 +1448,22 @@
     </row>
     <row r="12" spans="1:9" ht="18.75">
       <c r="A12" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G12" s="3">
         <v>5</v>
@@ -1435,24 +1471,24 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="18.75">
+    <row r="13" spans="1:9" ht="37.5">
       <c r="A13" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>103</v>
+        <v>93</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G13" s="3">
         <v>5</v>
@@ -1462,22 +1498,22 @@
     </row>
     <row r="14" spans="1:9" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G14" s="3">
         <v>4</v>
@@ -1496,9 +1532,9 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="18.75">
+    <row r="16" spans="1:9" ht="37.5">
       <c r="A16" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
@@ -1506,14 +1542,14 @@
       <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>29</v>
+      <c r="D16" s="15" t="s">
+        <v>174</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G16" s="3">
         <v>5</v>
@@ -1523,7 +1559,7 @@
     </row>
     <row r="17" spans="1:9" ht="18.75">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
@@ -1535,10 +1571,10 @@
         <v>28</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G17" s="3">
         <v>5</v>
@@ -1548,7 +1584,7 @@
     </row>
     <row r="18" spans="1:9" ht="18.75">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
@@ -1560,10 +1596,10 @@
         <v>22</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G18" s="3">
         <v>3</v>
@@ -1571,9 +1607,9 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" ht="18.75">
+    <row r="19" spans="1:9" ht="37.5">
       <c r="A19" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
@@ -1581,14 +1617,14 @@
       <c r="C19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>112</v>
+      <c r="D19" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G19" s="3">
         <v>3</v>
@@ -1598,7 +1634,7 @@
     </row>
     <row r="20" spans="1:9" ht="18.75">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
@@ -1607,13 +1643,13 @@
         <v>20</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G20" s="3">
         <v>1</v>
@@ -1623,22 +1659,22 @@
     </row>
     <row r="21" spans="1:9" ht="18.75">
       <c r="A21" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G21" s="3">
         <v>4</v>
@@ -1648,22 +1684,22 @@
     </row>
     <row r="22" spans="1:9" ht="18.75">
       <c r="A22" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G22" s="3">
         <v>4</v>
@@ -1684,7 +1720,7 @@
     </row>
     <row r="24" spans="1:9" ht="18.75">
       <c r="A24" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
@@ -1696,22 +1732,22 @@
         <v>23</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G24" s="3">
         <v>5</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="7" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18.75">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>10</v>
@@ -1723,10 +1759,10 @@
         <v>26</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G25" s="3">
         <v>5</v>
@@ -1736,7 +1772,7 @@
     </row>
     <row r="26" spans="1:9" ht="18.75">
       <c r="A26" s="8" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>10</v>
@@ -1745,13 +1781,13 @@
         <v>14</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G26" s="7">
         <v>5</v>
@@ -1761,7 +1797,7 @@
     </row>
     <row r="27" spans="1:9" ht="18.75">
       <c r="A27" s="8" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>10</v>
@@ -1770,13 +1806,13 @@
         <v>14</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G27" s="7">
         <v>5</v>
@@ -1786,7 +1822,7 @@
     </row>
     <row r="28" spans="1:9" ht="18.75">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>10</v>
@@ -1798,10 +1834,10 @@
         <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G28" s="3">
         <v>5</v>
@@ -1811,7 +1847,7 @@
     </row>
     <row r="29" spans="1:9" ht="18.75">
       <c r="A29" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>10</v>
@@ -1820,13 +1856,13 @@
         <v>14</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G29" s="3">
         <v>3</v>
@@ -1836,7 +1872,7 @@
     </row>
     <row r="30" spans="1:9" ht="18.75">
       <c r="A30" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>10</v>
@@ -1845,13 +1881,13 @@
         <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G30" s="3">
         <v>5</v>
@@ -1861,7 +1897,7 @@
     </row>
     <row r="31" spans="1:9" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>10</v>
@@ -1870,13 +1906,13 @@
         <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G31" s="3">
         <v>3</v>
@@ -1886,7 +1922,7 @@
     </row>
     <row r="32" spans="1:9" ht="18.75">
       <c r="A32" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>10</v>
@@ -1895,13 +1931,13 @@
         <v>15</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G32" s="3">
         <v>5</v>
@@ -1911,7 +1947,7 @@
     </row>
     <row r="33" spans="1:9" ht="18.75">
       <c r="A33" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>10</v>
@@ -1923,10 +1959,10 @@
         <v>25</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G33" s="3">
         <v>3</v>
@@ -1936,7 +1972,7 @@
     </row>
     <row r="34" spans="1:9" ht="18.75">
       <c r="A34" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>10</v>
@@ -1945,13 +1981,13 @@
         <v>15</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G34" s="3">
         <v>4</v>
@@ -1972,7 +2008,7 @@
     </row>
     <row r="36" spans="1:9" ht="18.75">
       <c r="A36" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
@@ -1981,13 +2017,13 @@
         <v>27</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="G36" s="3">
         <v>5</v>
@@ -1997,7 +2033,7 @@
     </row>
     <row r="37" spans="1:9" ht="18.75">
       <c r="A37" s="8" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>11</v>
@@ -2006,13 +2042,13 @@
         <v>27</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G37" s="3">
         <v>5</v>
@@ -2022,7 +2058,7 @@
     </row>
     <row r="38" spans="1:9" ht="18.75">
       <c r="A38" s="8" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>11</v>
@@ -2031,13 +2067,13 @@
         <v>27</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G38" s="3">
         <v>5</v>
@@ -2045,9 +2081,9 @@
       <c r="H38" s="9"/>
       <c r="I38" s="7"/>
     </row>
-    <row r="39" spans="1:9" ht="18.75">
+    <row r="39" spans="1:9" ht="37.5">
       <c r="A39" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>11</v>
@@ -2055,14 +2091,14 @@
       <c r="C39" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>43</v>
+      <c r="D39" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G39" s="3">
         <v>5</v>
@@ -2072,7 +2108,7 @@
     </row>
     <row r="40" spans="1:9" ht="18.75">
       <c r="A40" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
@@ -2081,13 +2117,13 @@
         <v>27</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G40" s="3">
         <v>4</v>
@@ -2095,9 +2131,9 @@
       <c r="H40" s="9"/>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" ht="18.75">
+    <row r="41" spans="1:9" ht="37.5">
       <c r="A41" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>11</v>
@@ -2105,14 +2141,14 @@
       <c r="C41" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>118</v>
+      <c r="D41" s="15" t="s">
+        <v>177</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G41" s="3">
         <v>4</v>
@@ -2120,24 +2156,24 @@
       <c r="H41" s="9"/>
       <c r="I41" s="7"/>
     </row>
-    <row r="42" spans="1:9" ht="18.75">
+    <row r="42" spans="1:9" ht="37.5">
       <c r="A42" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G42" s="3">
         <v>4</v>
@@ -2147,22 +2183,22 @@
     </row>
     <row r="43" spans="1:9" ht="18.75">
       <c r="A43" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G43" s="3">
         <v>4</v>
@@ -2170,9 +2206,9 @@
       <c r="H43" s="9"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="18.75">
+    <row r="44" spans="1:9" ht="37.5">
       <c r="A44" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>11</v>
@@ -2180,14 +2216,14 @@
       <c r="C44" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>92</v>
+      <c r="D44" s="15" t="s">
+        <v>179</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G44" s="3">
         <v>2</v>
@@ -2197,22 +2233,22 @@
     </row>
     <row r="45" spans="1:9" ht="18.75">
       <c r="A45" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G45" s="3">
         <v>4</v>
@@ -2231,9 +2267,9 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="47" spans="1:9" ht="18.75">
+    <row r="47" spans="1:9" ht="37.5">
       <c r="A47" s="13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>17</v>
@@ -2241,14 +2277,14 @@
       <c r="C47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>150</v>
+      <c r="D47" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="G47" s="3">
         <v>5</v>
@@ -2256,7 +2292,7 @@
     </row>
     <row r="48" spans="1:9" ht="18.75">
       <c r="A48" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>17</v>
@@ -2265,22 +2301,22 @@
         <v>18</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G48" s="3">
         <v>4</v>
       </c>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="18.75">
+    <row r="49" spans="1:7" ht="37.5">
       <c r="A49" s="13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>17</v>
@@ -2288,14 +2324,14 @@
       <c r="C49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>151</v>
+      <c r="D49" s="15" t="s">
+        <v>181</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G49" s="3">
         <v>4</v>
@@ -2303,7 +2339,7 @@
     </row>
     <row r="50" spans="1:7" ht="18.75">
       <c r="A50" s="13" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>17</v>
@@ -2312,21 +2348,21 @@
         <v>18</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G50" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="18.75">
+    <row r="51" spans="1:7" ht="56.25">
       <c r="A51" s="13" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>17</v>
@@ -2334,22 +2370,22 @@
       <c r="C51" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>153</v>
+      <c r="D51" s="15" t="s">
+        <v>182</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G51" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="18.75">
+    <row r="52" spans="1:7" ht="37.5">
       <c r="A52" s="13" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>17</v>
@@ -2357,22 +2393,22 @@
       <c r="C52" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>164</v>
+      <c r="D52" s="15" t="s">
+        <v>183</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G52" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="18.75">
+    <row r="53" spans="1:7" ht="37.5">
       <c r="A53" s="13" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>17</v>
@@ -2380,37 +2416,37 @@
       <c r="C53" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>167</v>
+      <c r="D53" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G53" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="18.75">
+    <row r="54" spans="1:7" ht="37.5">
       <c r="A54" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>45</v>
+        <v>31</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G54" s="3">
         <v>3</v>
@@ -2418,22 +2454,22 @@
     </row>
     <row r="55" spans="1:7" ht="18.75">
       <c r="A55" s="13" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G55" s="3">
         <v>4</v>
@@ -2441,45 +2477,45 @@
     </row>
     <row r="56" spans="1:7" ht="18.75">
       <c r="A56" s="13" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G56" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="18.75">
+    <row r="57" spans="1:7" ht="37.5">
       <c r="A57" s="13" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>162</v>
+        <v>140</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>186</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G57" s="3">
         <v>3</v>
@@ -2487,22 +2523,22 @@
     </row>
     <row r="58" spans="1:7" ht="18.75">
       <c r="A58" s="13" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G58" s="3">
         <v>3</v>
@@ -2510,22 +2546,22 @@
     </row>
     <row r="59" spans="1:7" ht="18.75">
       <c r="A59" s="13" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F59" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G59" s="3">
         <v>3</v>
@@ -2533,22 +2569,22 @@
     </row>
     <row r="60" spans="1:7" ht="18.75">
       <c r="A60" s="13" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F60" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="G60" s="3">
         <v>3</v>
@@ -2565,22 +2601,22 @@
     </row>
     <row r="62" spans="1:7" ht="18.75">
       <c r="A62" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G62" s="3">
         <v>5</v>
@@ -2588,22 +2624,22 @@
     </row>
     <row r="63" spans="1:7" ht="18.75">
       <c r="A63" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G63" s="3">
         <v>5</v>
@@ -2611,22 +2647,22 @@
     </row>
     <row r="64" spans="1:7" ht="18.75">
       <c r="A64" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="G64" s="3">
         <v>3</v>
@@ -2642,22 +2678,22 @@
     </row>
     <row r="66" spans="1:7" ht="18.75">
       <c r="A66" s="13" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G66" s="3">
         <v>5</v>
@@ -2665,60 +2701,74 @@
     </row>
     <row r="67" spans="1:7" ht="18.75">
       <c r="A67" s="13" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="G67" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18.75">
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-    </row>
-    <row r="69" spans="1:7" ht="18.75">
+      <c r="A68" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G68" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="37.5">
       <c r="A69" s="13" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>147</v>
+        <v>131</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>187</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="G69" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18.75">
-      <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2728,85 +2778,117 @@
     </row>
     <row r="71" spans="1:7" ht="18.75">
       <c r="A71" s="13" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>175</v>
+        <v>133</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="G71" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18.75">
-      <c r="A72" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G72" s="3">
-        <v>3</v>
-      </c>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="18.75">
       <c r="A73" s="13" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="G73" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18.75">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
+      <c r="A74" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G74" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="18.75">
+      <c r="A75" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="G75" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="18.75">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>